<commit_message>
fix extractor + added test
</commit_message>
<xml_diff>
--- a/TESTFILEMETDATA.xlsx
+++ b/TESTFILEMETDATA.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">t             </t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Som X</t>
+  </si>
+  <si>
+    <t>STDDev X</t>
   </si>
 </sst>
 </file>
@@ -412,7 +415,7 @@
   <dimension ref="A1:I1100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +549,13 @@
       </c>
       <c r="D7">
         <v>-0.27532840380000001</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <f>STDEV(B2:B1100)</f>
+        <v>3.0718109575773638</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>